<commit_message>
Update sheets related to Test Plan/Design updates of chapter 5
</commit_message>
<xml_diff>
--- a/ATDD Scenarios/Clean sheet.xlsx
+++ b/ATDD Scenarios/Clean sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\source\repos\Automated-Testing-in-Microsoft-Dynamics-365-Business-Central-Second-Edition\ATDD Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571856EC-61F1-4997-BE8F-1AF79A0DEDB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE4FA88-D98D-41FF-B149-4C5435FAD60C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{DB99ADC0-1D36-4CB0-890F-ABAEDD9356F9}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
@@ -295,6 +295,88 @@
   </cellStyles>
   <dxfs count="30">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -358,47 +440,6 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -460,47 +501,6 @@
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0070C0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -515,54 +515,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L6" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D77B0683-CDBE-450E-913A-81EFBBA8B17E}" name="Table2" displayName="Table2" ref="A1:L6" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:L6" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{8363E7FF-10AC-4A2B-AF58-2B6F4A3A2982}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{47ED26B9-CBC1-4AA1-A3A9-843BF13AA89B}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{42186982-BEE2-4B88-B732-989CDBD8F258}" name="Positive-negative" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{2CFDA2E7-B629-4ECF-BE79-854343648AF6}" name="UI" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{42186982-BEE2-4B88-B732-989CDBD8F258}" name="Positive-negative" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{CF058E75-EBE8-492F-899F-08E1336AACB4}" name="Scenario" dataDxfId="26"/>
     <tableColumn id="3" xr3:uid="{824F4994-529B-42E7-960A-C52362C8177D}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{9A2C2A27-BDEF-4BD0-8B83-E6DCBCFA35E2}" name="Given-When-Then (Description)" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{357E2CE4-1423-477D-9378-4140E6CC741F}" name="Scenario #" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{A0EF38BD-226F-4389-8485-98738BF5C0B4}" name="ATDD Format" dataDxfId="23">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{55990E10-8959-4AC5-A765-C7364ECDCDE5}" name="Code Format" dataDxfId="22">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="16">
+    <tableColumn id="11" xr3:uid="{428C58FA-6B63-4AB1-8578-57C5373BC837}" name="ATDD.TestScriptor Format" dataDxfId="21">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{67272D7F-D0CB-4C6B-967E-B47CC34979CB}" name="Notes" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L18" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:L18" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC94DC61-3A21-44B1-A4FA-D3AE0A291830}" name="Table23" displayName="Table23" ref="A1:L17" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A1:L17" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{EB12FABE-99EE-4C64-9371-664DA2BC018B}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{C4BF811B-A50B-4F15-ABFB-76F5EF61BAEC}" name="Sub Feature"/>
-    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{050332A6-04F7-4C80-8BF0-1A37BF66834D}" name="UI" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{91F463C5-D5E2-4E74-89F7-26421CFD4688}" name="Positive-negative" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{F4B03F80-242C-48F3-AD45-4F8870F7CF4C}" name="Scenario" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{CC6D9ED1-342A-442A-A781-19E1B48EC192}" name="Given-When-Then (Tag)"/>
-    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{4B77C75B-29B6-4D6D-8295-8BCB00B5A021}" name="Given-When-Then (Description)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{7A8CEFC7-AFDE-40F5-BF03-D453506926E6}" name="Scenario #" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{4C548BB4-BEA7-4564-81EF-9BD6BCF666EF}" name="ATDD Format" dataDxfId="13">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{762A89F1-1CE0-4623-9ECE-7E18ABCC76DC}" name="Code Format" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{01376FDB-C35B-4080-A02C-72B0C39BDC01}" name="ATDD.TestScriptor Format" dataDxfId="11">
       <calculatedColumnFormula>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{108458B0-953E-40C3-A10B-F57A3E16C1B8}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08B1ED69-5F96-4A81-993F-0E906F475813}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,7 +887,7 @@
     <col min="12" max="12" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,25 +925,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="I2" s="7" t="str">
+      <c r="B2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="str">
         <f>IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table2[[#This Row],[Feature]]," ",Table2[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table2[[#This Row],[Scenario '#]],"0000"),"] ",Table2[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table2[[#This Row],[Given-When-Then (Tag)]]),"] ",Table2[[#This Row],[Given-When-Then (Description)]]))</f>
         <v xml:space="preserve">[FEATURE] Feature </v>
       </c>
-      <c r="J2" s="7" t="str">
+      <c r="J2" s="11" t="str">
         <f>_xlfn.CONCAT("//",Table2[[#This Row],[ATDD Format]])</f>
         <v xml:space="preserve">//[FEATURE] Feature </v>
       </c>
-      <c r="K2" s="17" t="str">
+      <c r="K2" s="18" t="str">
         <f ca="1">IF(Table2[[#This Row],[Given-When-Then (Tag)]]="",IF(Table2[[#This Row],[Scenario]]="",IF(Table2[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table2[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table2[[#This Row],[Scenario '#]],"0000")," '",Table2[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table2[[#This Row],[Given-When-Then (Tag)]]," '",Table2[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'Feature' {</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1055,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:D1048576">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1063,18 +1072,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1088,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9C69E6-B7EF-4C82-A3EA-E6EE3FD2884C}">
-  <dimension ref="A1:L109"/>
+  <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1117,7 @@
     <col min="12" max="12" width="47.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1146,80 +1155,91 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="I2" s="7" t="str">
-        <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v xml:space="preserve">[FEATURE] Label UT </v>
-      </c>
-      <c r="J2" s="14" t="str">
-        <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v xml:space="preserve">//[FEATURE] Label UT </v>
-      </c>
-      <c r="K2" s="17" t="str">
-        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Feature 'Label UT ' {</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="21" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="11" t="str">
+      <c r="H2" s="12"/>
+      <c r="I2" s="11" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[FEATURE] Label UT Customer</v>
       </c>
-      <c r="J3" s="13" t="str">
+      <c r="J2" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
         <v>//[FEATURE] Label UT Customer</v>
       </c>
-      <c r="K3" s="18" t="str">
+      <c r="K2" s="18" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Feature 'Label UT Customer' {</v>
       </c>
-      <c r="L3" s="11"/>
-    </row>
-    <row r="4" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0001] Check that label can be assigned to customer</v>
+      </c>
+      <c r="J3" s="14" t="str">
+        <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0001] Check that label can be assigned to customer</v>
+      </c>
+      <c r="K3" s="17" t="str">
+        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0001 'Check that label can be assigned to customer' {</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="H4" s="8">
         <v>1</v>
       </c>
       <c r="I4" s="7" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0001] Check that label can be assigned to customer</v>
+        <v>[GIVEN] A label</v>
       </c>
       <c r="J4" s="14" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0001] Check that label can be assigned to customer</v>
+        <v>//[GIVEN] A label</v>
       </c>
       <c r="K4" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0001 'Check that label can be assigned to customer' {</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>13</v>
+        <v>Given 'A label'</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1233,22 +1253,22 @@
         <v>14</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="8">
         <v>1</v>
       </c>
       <c r="I5" s="7" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A label</v>
+        <v>[GIVEN] A customer</v>
       </c>
       <c r="J5" s="14" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A label</v>
+        <v>//[GIVEN] A customer</v>
       </c>
       <c r="K5" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A label'</v>
+        <v>Given 'A customer'</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1259,28 +1279,28 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
       </c>
       <c r="I6" s="7" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A customer</v>
+        <v>[WHEN] Assign label to customer</v>
       </c>
       <c r="J6" s="14" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A customer</v>
+        <v>//[WHEN] Assign label to customer</v>
       </c>
       <c r="K6" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A customer'</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>When 'Assign label to customer'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1288,80 +1308,80 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="I7" s="7" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Assign label to customer</v>
+        <v>[THEN] Customer has label field populated</v>
       </c>
       <c r="J7" s="14" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Assign label to customer</v>
+        <v>//[THEN] Customer has label field populated</v>
       </c>
       <c r="K7" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Assign label to customer'</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+        <v>Then 'Customer has label field populated' }</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>20</v>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7" t="str">
+        <v>2</v>
+      </c>
+      <c r="I8" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Customer has label field populated</v>
-      </c>
-      <c r="J8" s="14" t="str">
+        <v>[SCENARIO #0002] Check that label field table relation is validated for non-existing label on customer</v>
+      </c>
+      <c r="J8" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Customer has label field populated</v>
+        <v>//[SCENARIO #0002] Check that label field table relation is validated for non-existing label on customer</v>
       </c>
       <c r="K8" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer has label field populated' }</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>Scenario 0002 'Check that label field table relation is validated for non-existing label on customer' {</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>21</v>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="8">
         <v>2</v>
       </c>
       <c r="I9" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0002] Check that label field table relation is validated for non-existing label on customer</v>
+        <v>[GIVEN] A non-existing label value</v>
       </c>
       <c r="J9" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0002] Check that label field table relation is validated for non-existing label on customer</v>
+        <v>//[GIVEN] A non-existing label value</v>
       </c>
       <c r="K9" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0002 'Check that label field table relation is validated for non-existing label on customer' {</v>
+        <v>Given 'A non-existing label value'</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1375,22 +1395,22 @@
         <v>14</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="I10" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A non-existing label value</v>
+        <v>[GIVEN] A customer record variable</v>
       </c>
       <c r="J10" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A non-existing label value</v>
+        <v>//[GIVEN] A customer record variable</v>
       </c>
       <c r="K10" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A non-existing label value'</v>
+        <v>Given 'A customer record variable'</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1401,28 +1421,28 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H11" s="8">
         <v>2</v>
       </c>
       <c r="I11" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A customer record variable</v>
+        <v>[WHEN] Assign non-existing label to customer</v>
       </c>
       <c r="J11" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A customer record variable</v>
+        <v>//[WHEN] Assign non-existing label to customer</v>
       </c>
       <c r="K11" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A customer record variable'</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>When 'Assign non-existing label to customer'</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1430,57 +1450,57 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H12" s="8">
         <v>2</v>
       </c>
       <c r="I12" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Assign non-existing label to customer</v>
+        <v>[THEN] Non existing label error was thrown</v>
       </c>
       <c r="J12" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Assign non-existing label to customer</v>
+        <v>//[THEN] Non existing label error was thrown</v>
       </c>
       <c r="K12" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Assign non-existing label to customer'</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+        <v>Then 'Non existing label error was thrown' }</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>25</v>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="H13" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Non existing label error was thrown</v>
+        <v>[SCENARIO #0003] Check that label can be assigned on customer card</v>
       </c>
       <c r="J13" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Non existing label error was thrown</v>
+        <v>//[SCENARIO #0003] Check that label can be assigned on customer card</v>
       </c>
       <c r="K13" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Non existing label error was thrown' }</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>Scenario 0003 'Check that label can be assigned on customer card' {</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1490,23 +1510,26 @@
       <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>27</v>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="H14" s="8">
         <v>3</v>
       </c>
       <c r="I14" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0003] Check that label can be assigned on customer card</v>
+        <v>[GIVEN] A label</v>
       </c>
       <c r="J14" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0003] Check that label can be assigned on customer card</v>
+        <v>//[GIVEN] A label</v>
       </c>
       <c r="K14" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0003 'Check that label can be assigned on customer card' {</v>
+        <v>Given 'A label'</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1523,22 +1546,22 @@
         <v>14</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H15" s="8">
         <v>3</v>
       </c>
       <c r="I15" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A label</v>
+        <v>[GIVEN] A customer card</v>
       </c>
       <c r="J15" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A label</v>
+        <v>//[GIVEN] A customer card</v>
       </c>
       <c r="K15" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A label'</v>
+        <v>Given 'A customer card'</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1552,28 +1575,28 @@
         <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H16" s="8">
         <v>3</v>
       </c>
       <c r="I16" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] A customer card</v>
+        <v>[WHEN] Assign label to customer card</v>
       </c>
       <c r="J16" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] A customer card</v>
+        <v>//[WHEN] Assign label to customer card</v>
       </c>
       <c r="K16" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'A customer card'</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>When 'Assign label to customer card'</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1584,64 +1607,32 @@
         <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H17" s="8">
         <v>3</v>
       </c>
       <c r="I17" s="15" t="str">
         <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Assign label to customer card</v>
+        <v>[THEN] Customer has label field populated</v>
       </c>
       <c r="J17" s="16" t="str">
         <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Assign label to customer card</v>
+        <v>//[THEN] Customer has label field populated</v>
       </c>
       <c r="K17" s="17" t="str">
         <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Assign label to customer card'</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="8">
-        <v>3</v>
-      </c>
-      <c r="I18" s="15" t="str">
-        <f>IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table23[[#This Row],[Scenario '#]],"0000"),"] ",Table23[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table23[[#This Row],[Given-When-Then (Tag)]]),"] ",Table23[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Customer has label field populated</v>
-      </c>
-      <c r="J18" s="16" t="str">
-        <f>_xlfn.CONCAT("//",Table23[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Customer has label field populated</v>
-      </c>
-      <c r="K18" s="17" t="str">
-        <f ca="1">IF(Table23[[#This Row],[Given-When-Then (Tag)]]="",IF(Table23[[#This Row],[Scenario]]="",IF(Table23[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table23[[#This Row],[Feature]]," ",Table23[[#This Row],[Sub Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table23[[#This Row],[Scenario '#]],"0000")," '",Table23[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table23[[#This Row],[Given-When-Then (Tag)]]," '",Table23[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Customer has label field populated' } }</v>
       </c>
     </row>
-    <row r="88" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1658,18 +1649,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>